<commit_message>
humidity offset should be SUBTRACTION
</commit_message>
<xml_diff>
--- a/observations.xlsx
+++ b/observations.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzarandi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heydaraliyev/async_flask/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3F6E6B4-6A4D-4965-8255-4B79C505FE19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9690E44-7F54-E045-9087-35321C045B41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{5FA52817-C69B-F448-B41E-B19221700329}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13620" xr2:uid="{5FA52817-C69B-F448-B41E-B19221700329}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -393,15 +388,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D188D8-33CC-2742-A1A3-B1791793C9A4}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,7 +410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>66</v>
       </c>
@@ -426,11 +421,11 @@
         <v>52</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D19" si="0">B2-C2</f>
+        <f t="shared" ref="D2:D20" si="0">B2-C2</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>67.540000000000006</v>
       </c>
@@ -445,7 +440,7 @@
         <v>5.7000000000000028</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>68.09</v>
       </c>
@@ -460,7 +455,7 @@
         <v>7.4399999999999977</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>66</v>
       </c>
@@ -475,7 +470,7 @@
         <v>0.53000000000000114</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>65.94</v>
       </c>
@@ -490,7 +485,7 @@
         <v>1.2899999999999991</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>67.52</v>
       </c>
@@ -505,7 +500,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>68.05</v>
       </c>
@@ -520,7 +515,7 @@
         <v>6.1500000000000057</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>68.180000000000007</v>
       </c>
@@ -535,7 +530,7 @@
         <v>6.4300000000000068</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>68.28</v>
       </c>
@@ -550,7 +545,7 @@
         <v>7.3400000000000034</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>67.150000000000006</v>
       </c>
@@ -565,7 +560,7 @@
         <v>4.2700000000000031</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>66.84</v>
       </c>
@@ -580,7 +575,7 @@
         <v>0.36999999999999744</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>67.39</v>
       </c>
@@ -595,7 +590,7 @@
         <v>7.1899999999999977</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>67.44</v>
       </c>
@@ -610,7 +605,7 @@
         <v>7.230000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>67.459999999999994</v>
       </c>
@@ -625,7 +620,7 @@
         <v>2.2100000000000009</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>67.8</v>
       </c>
@@ -640,7 +635,7 @@
         <v>3.7999999999999972</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>68.5</v>
       </c>
@@ -655,7 +650,7 @@
         <v>3.7899999999999991</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>69.400000000000006</v>
       </c>
@@ -670,7 +665,7 @@
         <v>7.8900000000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>69.47</v>
       </c>
@@ -683,6 +678,18 @@
       <c r="D19">
         <f t="shared" si="0"/>
         <v>5.4300000000000068</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>52.76</v>
+      </c>
+      <c r="C20">
+        <v>51</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1.759999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>